<commit_message>
introdução do vue e def compara() retornando resultados de acordo com o esperado
</commit_message>
<xml_diff>
--- a/uploads/Planilha1.xlsx
+++ b/uploads/Planilha1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pax Primavera\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pax Primavera\Documents\MeusProjetos\Projeto_Vendas\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56289DF0-407D-484D-8B96-C171C4730395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAC7F93-BB53-4BAC-BEA6-6C79030B3DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B6058359-1EB6-4608-AECD-5D4CE26AD963}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B6058359-1EB6-4608-AECD-5D4CE26AD963}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendas" sheetId="2" r:id="rId1"/>
@@ -4848,7 +4848,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{330AE7F0-F18B-4DDB-814F-44916A3B1CA3}">
   <dimension ref="A1:U571"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>